<commit_message>
Processing corrected to exclude rouge subject names
	-- Some experimentation with the open AI API.
</commit_message>
<xml_diff>
--- a/output/Intermediate_2_2001.xlsx
+++ b/output/Intermediate_2_2001.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E135"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1983,15 +1983,15 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - as percentages</t>
+          <t>Classical Greek</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2006,11 +2006,11 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Classical Greek</t>
+          <t>English and Communication</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>7</v>
+        <v>5417</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2029,11 +2029,11 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>English and Communication</t>
+          <t>French</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>5417</v>
+        <v>701</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2052,11 +2052,11 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>French</t>
+          <t>Gaelic (Learners)</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>701</v>
+        <v>8</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2075,11 +2075,11 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Gaelic (Learners)</t>
+          <t>Gàidhlig</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2098,11 +2098,11 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Gàidhlig</t>
+          <t>German</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>4</v>
+        <v>323</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2121,11 +2121,11 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>German</t>
+          <t>Italian</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>323</v>
+        <v>102</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2144,11 +2144,11 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Italian</t>
+          <t>Latin</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>102</v>
+        <v>6</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2167,11 +2167,13 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Latin</t>
-        </is>
-      </c>
-      <c r="B76" t="n">
-        <v>6</v>
+          <t>Russian</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2190,13 +2192,11 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Russian</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>269</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2215,11 +2215,11 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Spanish</t>
+          <t>Accounting and Finance</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>269</v>
+        <v>301</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2238,11 +2238,11 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Accounting and Finance</t>
+          <t>Mathematics</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>301</v>
+        <v>5886</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2261,11 +2261,11 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Mathematics</t>
+          <t>Biology</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>5886</v>
+        <v>2418</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2284,11 +2284,11 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Biology</t>
+          <t>Biotechnology</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>2418</v>
+        <v>39</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2307,11 +2307,11 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Biotechnology</t>
+          <t>Chemistry</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>39</v>
+        <v>775</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2330,11 +2330,11 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Geology</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>775</v>
+        <v>5</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2353,11 +2353,11 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Geology</t>
+          <t>Managing Environmental Resources</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2376,11 +2376,11 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Managing Environmental Resources</t>
+          <t>Physics</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>20</v>
+        <v>454</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2399,11 +2399,11 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>Amenity Horticulture</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>454</v>
+        <v>13</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2422,11 +2422,13 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Amenity Horticulture</t>
-        </is>
-      </c>
-      <c r="B87" t="n">
-        <v>13</v>
+          <t>Crop Establishment</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2445,7 +2447,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Crop Establishment</t>
+          <t>Fish Husbandry</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2470,7 +2472,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Fish Husbandry</t>
+          <t>Investigating Fish Rearing Systems</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2495,7 +2497,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Investigating Fish Rearing Systems</t>
+          <t>Livestock Production</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2520,13 +2522,11 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Livestock Production</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>Plant Propagation</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>13</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2545,11 +2545,11 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Plant Propagation</t>
+          <t>Classical Studies</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2568,11 +2568,11 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Classical Studies</t>
+          <t>Economics</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2591,11 +2591,11 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Economics</t>
+          <t>Geography</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>77</v>
+        <v>507</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2614,11 +2614,11 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Geography</t>
+          <t>History</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>507</v>
+        <v>844</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2637,11 +2637,11 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>History</t>
+          <t>Modern Studies</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>844</v>
+        <v>629</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -2660,11 +2660,11 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Modern Studies</t>
+          <t>Philosophy</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>629</v>
+        <v>32</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
@@ -2683,11 +2683,11 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Philosophy</t>
+          <t>Psychology</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>32</v>
+        <v>194</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
@@ -2706,11 +2706,11 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Psychology</t>
+          <t>Religious, Moral and Philosophical Studies</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
@@ -2729,11 +2729,11 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Religious, Moral and Philosophical Studies</t>
+          <t>Sociology</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>187</v>
+        <v>97</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
@@ -2752,11 +2752,11 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Sociology</t>
+          <t>Administration</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>97</v>
+        <v>2238</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
@@ -2775,11 +2775,11 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Administration</t>
+          <t>Business Management</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>2238</v>
+        <v>607</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
@@ -2798,11 +2798,11 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Business Management</t>
+          <t>Care</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>607</v>
+        <v>296</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
@@ -2821,11 +2821,11 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Care</t>
+          <t>Care Issues for Society</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>296</v>
+        <v>109</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
@@ -2844,11 +2844,11 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Care Issues for Society</t>
+          <t>Computing</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>109</v>
+        <v>522</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
@@ -2867,11 +2867,13 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Computing</t>
-        </is>
-      </c>
-      <c r="B106" t="n">
-        <v>522</v>
+          <t>Construction Craft Skills</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
@@ -2890,7 +2892,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Construction Craft Skills</t>
+          <t>Construction Industry Practice</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -2915,13 +2917,11 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Construction Industry Practice</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>Craft and Design</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>135</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
@@ -2940,11 +2940,11 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Craft and Design</t>
+          <t>Design</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>135</v>
+        <v>33</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
@@ -2963,11 +2963,11 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Design</t>
+          <t>Electronic and Electrical Fundamentals</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
@@ -2986,11 +2986,11 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Electronic and Electrical Fundamentals</t>
+          <t>Engineering Craft Skills</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
@@ -3009,11 +3009,13 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Engineering Craft Skills</t>
-        </is>
-      </c>
-      <c r="B112" t="n">
-        <v>7</v>
+          <t>Fabrication and Welding</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
@@ -3032,13 +3034,11 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Fabrication and Welding</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>Graphic Communication</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>223</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
@@ -3057,11 +3057,11 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Graphic Communication</t>
+          <t>Health and Safety in Care Settings</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>223</v>
+        <v>41</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
@@ -3080,7 +3080,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Health and Safety in Care Settings</t>
+          <t>Home Economics - Fashion and Textile Technology</t>
         </is>
       </c>
       <c r="B115" t="n">
@@ -3103,11 +3103,11 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Home Economics - Fashion and Textile Technology</t>
+          <t>Home Economics - Health and Food Technology</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>41</v>
+        <v>238</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
@@ -3126,11 +3126,11 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Home Economics - Health and Food Technology</t>
+          <t>Home Economics - Lifestyle and Consumer Technology</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>238</v>
+        <v>47</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
@@ -3149,11 +3149,11 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Home Economics - Lifestyle and Consumer Technology</t>
+          <t>Hospitality - General Operations</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
@@ -3172,11 +3172,11 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Hospitality - General Operations</t>
+          <t>Hospitality - Practical Cookery</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>103</v>
+        <v>1545</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
@@ -3195,11 +3195,11 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Hospitality - Practical Cookery</t>
+          <t>Hospitality - Professional Cookery</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>1545</v>
+        <v>97</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
@@ -3218,11 +3218,11 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Hospitality - Professional Cookery</t>
+          <t>Information Systems</t>
         </is>
       </c>
       <c r="B121" t="n">
-        <v>97</v>
+        <v>1123</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
@@ -3241,11 +3241,11 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Information Systems</t>
+          <t>Personal and Social Education</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>1123</v>
+        <v>22</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
@@ -3264,11 +3264,11 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Personal and Social Education</t>
+          <t>Selling Overseas Tourist Destinations</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
@@ -3287,11 +3287,11 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Selling Overseas Tourist Destinations</t>
+          <t>Technological Studies</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
@@ -3310,11 +3310,11 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Technological Studies</t>
+          <t>Travel and Tourism</t>
         </is>
       </c>
       <c r="B125" t="n">
-        <v>2</v>
+        <v>437</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
@@ -3333,11 +3333,11 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Travel and Tourism</t>
+          <t>Woodworking Skills</t>
         </is>
       </c>
       <c r="B126" t="n">
-        <v>437</v>
+        <v>247</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
@@ -3356,11 +3356,11 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Woodworking Skills</t>
+          <t>Art and Design</t>
         </is>
       </c>
       <c r="B127" t="n">
-        <v>247</v>
+        <v>1063</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
@@ -3379,11 +3379,11 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Art and Design</t>
+          <t>Drama</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>1063</v>
+        <v>312</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
@@ -3402,11 +3402,11 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Media Studies</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>312</v>
+        <v>245</v>
       </c>
       <c r="C129" t="inlineStr">
         <is>
@@ -3425,11 +3425,11 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Media Studies</t>
+          <t>Music</t>
         </is>
       </c>
       <c r="B130" t="n">
-        <v>245</v>
+        <v>382</v>
       </c>
       <c r="C130" t="inlineStr">
         <is>
@@ -3448,11 +3448,11 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Music</t>
+          <t>Fitness and Exercise</t>
         </is>
       </c>
       <c r="B131" t="n">
-        <v>382</v>
+        <v>4</v>
       </c>
       <c r="C131" t="inlineStr">
         <is>
@@ -3471,11 +3471,11 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Fitness and Exercise</t>
+          <t>Leading Sports Activities</t>
         </is>
       </c>
       <c r="B132" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
@@ -3494,11 +3494,11 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Leading Sports Activities</t>
+          <t>Physical Education</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>5</v>
+        <v>416</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
@@ -3509,52 +3509,6 @@
         <v>2001</v>
       </c>
       <c r="E133" t="inlineStr">
-        <is>
-          <t>Intermediate_2</t>
-        </is>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>Physical Education</t>
-        </is>
-      </c>
-      <c r="B134" t="n">
-        <v>416</v>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="D134" t="n">
-        <v>2001</v>
-      </c>
-      <c r="E134" t="inlineStr">
-        <is>
-          <t>Intermediate_2</t>
-        </is>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - as percentages</t>
-        </is>
-      </c>
-      <c r="B135" t="n">
-        <v>1</v>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="D135" t="n">
-        <v>2001</v>
-      </c>
-      <c r="E135" t="inlineStr">
         <is>
           <t>Intermediate_2</t>
         </is>

</xml_diff>